<commit_message>
Updated BOM to reflect correct 10 pin header
</commit_message>
<xml_diff>
--- a/Modules/SensorBug/v1/sensorbug_BOM.xlsx
+++ b/Modules/SensorBug/v1/sensorbug_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinandsukumar/Documents/Drive/agr_summer_2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinandsukumar/Drive/agr_summer_2017/LoRaBug/Modules/SensorBug/v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -125,9 +125,6 @@
     <t>10 pin 1.27mm Female Header</t>
   </si>
   <si>
-    <t>M50-3100545</t>
-  </si>
-  <si>
     <t>Harwin, Inc</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>RC0603JR-0720RL</t>
+  </si>
+  <si>
+    <t>M50-3120545</t>
   </si>
 </sst>
 </file>
@@ -251,6 +251,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -557,7 +558,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,10 +765,10 @@
         <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -778,13 +779,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -795,13 +796,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" t="s">
         <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -812,13 +813,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -829,13 +830,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -846,13 +847,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -863,13 +864,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -880,13 +881,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" t="s">
         <v>51</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -897,13 +898,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" t="s">
         <v>54</v>
-      </c>
-      <c r="D20" t="s">
-        <v>55</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -914,13 +915,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -931,13 +932,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -948,13 +949,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -965,13 +966,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -982,13 +983,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25">
         <v>1</v>

</xml_diff>